<commit_message>
switch in the G&C (2003) reading
</commit_message>
<xml_diff>
--- a/BBC-overview.xlsx
+++ b/BBC-overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcasillas/Documents/GitHub/chatterlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8AA35A-89FC-024F-834E-E640726D3933}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C4A4B3-3CD5-B641-8DAD-740A87A606B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,9 +180,6 @@
     <t>Kuhl et al. (2003)</t>
   </si>
   <si>
-    <t>Gergely et al. (2007)</t>
-  </si>
-  <si>
     <t>Scholl &amp; Tremoulet (2000)</t>
   </si>
   <si>
@@ -271,6 +268,9 @@
   </si>
   <si>
     <t>Headcam (Bergelson–confirmed), sleep studies (Frost)</t>
+  </si>
+  <si>
+    <t>Gergely &amp; Csibra (2003)</t>
   </si>
 </sst>
 </file>
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1007,7 +1007,7 @@
         <v>7</v>
       </c>
       <c r="L1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1021,7 +1021,7 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
         <v>27</v>
@@ -1054,13 +1054,13 @@
         <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>60</v>
-      </c>
       <c r="H3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K3" s="6"/>
     </row>
@@ -1081,13 +1081,13 @@
         <v>13</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K4" s="6"/>
     </row>
@@ -1119,10 +1119,10 @@
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1175,10 +1175,10 @@
         <v>51</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="K7" s="6"/>
     </row>
@@ -1300,10 +1300,10 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -1323,13 +1323,13 @@
         <v>23</v>
       </c>
       <c r="F12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="J12" t="s">
         <v>26</v>
@@ -1353,13 +1353,13 @@
         <v>28</v>
       </c>
       <c r="F13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="K13" s="6"/>
     </row>
@@ -1393,10 +1393,10 @@
         <v>26</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1416,13 +1416,13 @@
         <v>25</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="I15" t="s">
         <v>14</v>
@@ -1476,13 +1476,13 @@
         <v>37</v>
       </c>
       <c r="F17" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="K17" s="6"/>
     </row>
@@ -1544,10 +1544,10 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add note about student planned absence
</commit_message>
<xml_diff>
--- a/BBC-overview.xlsx
+++ b/BBC-overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcasillas/Documents/GitHub/chatterlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5238E3E6-28D4-B248-BF83-165B984B5B1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4854F41-D667-1746-8BE9-B38EC1C4FABC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33400" yWindow="-5560" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BBC-overview.csv" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="84">
   <si>
     <t>Week</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>Smith et al. (2018)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>EH exam in other course</t>
   </si>
 </sst>
 </file>
@@ -955,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -972,7 +978,7 @@
     <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1009,8 +1015,11 @@
       <c r="L1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1037,7 +1046,7 @@
       </c>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1064,7 +1073,7 @@
       </c>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1091,7 +1100,7 @@
       </c>
       <c r="K4" s="6"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1125,7 +1134,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1155,7 +1164,7 @@
       </c>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1182,7 +1191,7 @@
       </c>
       <c r="K7" s="6"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1212,7 +1221,7 @@
       </c>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1241,8 +1250,11 @@
         <v>14</v>
       </c>
       <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1272,7 +1284,7 @@
       </c>
       <c r="K10" s="6"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>5</v>
       </c>
@@ -1306,7 +1318,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>6</v>
       </c>
@@ -1336,7 +1348,7 @@
       </c>
       <c r="K12" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1363,7 +1375,7 @@
       </c>
       <c r="K13" s="6"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1399,7 +1411,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1428,8 +1440,11 @@
         <v>14</v>
       </c>
       <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
add CS as guest
</commit_message>
<xml_diff>
--- a/BBC-overview.xlsx
+++ b/BBC-overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcasillas/Documents/GitHub/chatterlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4466A935-FB42-8D48-B64D-813963626E0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA10F834-0FEB-1D4F-B333-D0E12102A69A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33400" yWindow="-5560" windowWidth="25600" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33400" yWindow="-5560" windowWidth="33400" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BBC-overview.csv" sheetId="1" r:id="rId1"/>
@@ -258,9 +258,6 @@
     <t>EEG (Snijders-confirmed), preferential head turn (Fikkert-confirmed)</t>
   </si>
   <si>
-    <t>Daylong audio (Cychosz-confirmed), multi-population comparison (Scaff)</t>
-  </si>
-  <si>
     <t>LWL (Weisleder-confirmed), CDI (Bergmann-confirmed), diary studies (Clark-confirmed)</t>
   </si>
   <si>
@@ -277,6 +274,9 @@
   </si>
   <si>
     <t>EH exam in other course</t>
+  </si>
+  <si>
+    <t>Daylong audio (Cychosz-confirmed), multi-population comparison (Scaff-confirmed)</t>
   </si>
 </sst>
 </file>
@@ -971,7 +971,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1023,7 +1023,7 @@
         <v>71</v>
       </c>
       <c r="M1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -1191,7 +1191,7 @@
         <v>51</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>52</v>
@@ -1258,7 +1258,7 @@
       </c>
       <c r="K9" s="6"/>
       <c r="M9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -1319,7 +1319,7 @@
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L11" t="s">
         <v>73</v>
@@ -1378,7 +1378,7 @@
         <v>68</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K13" s="6"/>
     </row>
@@ -1412,7 +1412,7 @@
         <v>26</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L14" t="s">
         <v>74</v>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="K15" s="6"/>
       <c r="M15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1566,7 +1566,7 @@
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="6" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="L19" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
add Mitchell & Jordan reading
</commit_message>
<xml_diff>
--- a/BBC-overview.xlsx
+++ b/BBC-overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcasillas/Documents/GitHub/chatterlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EA3715-7686-1F46-B289-3210C11453F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE4BCD51-0E7D-074B-8257-034B639A78AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36280" yWindow="-6340" windowWidth="33400" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -276,7 +276,7 @@
     <t>Headcam (Bergelson–confirmed), LWL (Weisleder-confirmed)</t>
   </si>
   <si>
-    <t>Mitchell &amp; Jordan (to appear)?</t>
+    <t>Mitchell &amp; Jordan (to appear)</t>
   </si>
 </sst>
 </file>
@@ -971,7 +971,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>